<commit_message>
resultado para el ipm global -SG
</commit_message>
<xml_diff>
--- a/Frecuentista_depto/COL/Output/smce_MC.xlsx
+++ b/Frecuentista_depto/COL/Output/smce_MC.xlsx
@@ -467,10 +467,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>0.00166768997407489</v>
+        <v>0.135675479443519</v>
       </c>
       <c r="C2" t="n">
-        <v>0.474569837575592</v>
+        <v>0.473842788633127</v>
       </c>
     </row>
     <row r="3">
@@ -478,10 +478,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>0.00205922044721979</v>
+        <v>0.135198094040841</v>
       </c>
       <c r="C3" t="n">
-        <v>0.46244953278094</v>
+        <v>0.460791351757007</v>
       </c>
     </row>
     <row r="4">
@@ -489,10 +489,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>0.00209658155137545</v>
+        <v>0.0581384868268255</v>
       </c>
       <c r="C4" t="n">
-        <v>0.279608049157258</v>
+        <v>0.279988761045496</v>
       </c>
     </row>
     <row r="5">
@@ -500,10 +500,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0016170427443921</v>
+        <v>0.215338968844249</v>
       </c>
       <c r="C5" t="n">
-        <v>0.636876305044764</v>
+        <v>0.632623940737174</v>
       </c>
     </row>
     <row r="6">
@@ -511,10 +511,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>0.00166569068645434</v>
+        <v>0.212810850633746</v>
       </c>
       <c r="C6" t="n">
-        <v>0.63075137314996</v>
+        <v>0.631192968656138</v>
       </c>
     </row>
     <row r="7">
@@ -522,10 +522,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0018159119181238</v>
+        <v>0.124448274891151</v>
       </c>
       <c r="C7" t="n">
-        <v>0.484654034470293</v>
+        <v>0.490201736805172</v>
       </c>
     </row>
     <row r="8">
@@ -533,10 +533,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>0.00154020937587433</v>
+        <v>0.191256596210678</v>
       </c>
       <c r="C8" t="n">
-        <v>0.777073375376594</v>
+        <v>0.774046143519458</v>
       </c>
     </row>
     <row r="9">
@@ -544,10 +544,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>0.00104130066209442</v>
+        <v>0.210623869643663</v>
       </c>
       <c r="C9" t="n">
-        <v>0.792447094300589</v>
+        <v>0.792234563204733</v>
       </c>
     </row>
     <row r="10">
@@ -555,10 +555,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>0.00186367717454543</v>
+        <v>0.229838728344693</v>
       </c>
       <c r="C10" t="n">
-        <v>0.661784220072395</v>
+        <v>0.659700510490542</v>
       </c>
     </row>
     <row r="11">
@@ -566,10 +566,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>0.00130330952652593</v>
+        <v>0.187851850948922</v>
       </c>
       <c r="C11" t="n">
-        <v>0.738264602039062</v>
+        <v>0.729332548739581</v>
       </c>
     </row>
     <row r="12">
@@ -577,10 +577,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="n">
-        <v>0.00403881517739169</v>
+        <v>0.158985275362944</v>
       </c>
       <c r="C12" t="n">
-        <v>0.479839529885194</v>
+        <v>0.481205105399773</v>
       </c>
     </row>
     <row r="13">
@@ -588,10 +588,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="n">
-        <v>0.000781012383408268</v>
+        <v>0.135650403714869</v>
       </c>
       <c r="C13" t="n">
-        <v>0.939174741961524</v>
+        <v>0.929001763996532</v>
       </c>
     </row>
     <row r="14">
@@ -599,10 +599,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="n">
-        <v>0.00183524823564586</v>
+        <v>0.199890021605445</v>
       </c>
       <c r="C14" t="n">
-        <v>0.621645731938332</v>
+        <v>0.633568644801997</v>
       </c>
     </row>
     <row r="15">
@@ -610,10 +610,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0011853080943816</v>
+        <v>0.182031513646177</v>
       </c>
       <c r="C15" t="n">
-        <v>0.82982049448968</v>
+        <v>0.829540995478474</v>
       </c>
     </row>
     <row r="16">
@@ -621,10 +621,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="n">
-        <v>0.00142828217770081</v>
+        <v>0.222696039185922</v>
       </c>
       <c r="C16" t="n">
-        <v>0.679526115331289</v>
+        <v>0.675641435518982</v>
       </c>
     </row>
     <row r="17">
@@ -632,10 +632,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="n">
-        <v>0.00178647089875053</v>
+        <v>0.198484683707293</v>
       </c>
       <c r="C17" t="n">
-        <v>0.586861278218917</v>
+        <v>0.585302236064272</v>
       </c>
     </row>
     <row r="18">
@@ -643,10 +643,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="n">
-        <v>0.00107816788148532</v>
+        <v>0.249156488427116</v>
       </c>
       <c r="C18" t="n">
-        <v>0.824782666571493</v>
+        <v>0.823820104523769</v>
       </c>
     </row>
     <row r="19">
@@ -654,10 +654,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="n">
-        <v>0.00183237861013552</v>
+        <v>0.200572948437639</v>
       </c>
       <c r="C19" t="n">
-        <v>0.6604056507232</v>
+        <v>0.659159066760244</v>
       </c>
     </row>
     <row r="20">
@@ -665,10 +665,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="n">
-        <v>0.00220207259274781</v>
+        <v>0.107189625075493</v>
       </c>
       <c r="C20" t="n">
-        <v>0.438517620467924</v>
+        <v>0.439344367434619</v>
       </c>
     </row>
     <row r="21">
@@ -676,10 +676,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="n">
-        <v>0.00218075151669395</v>
+        <v>0.0940485505915715</v>
       </c>
       <c r="C21" t="n">
-        <v>0.46111164389625</v>
+        <v>0.463658576529257</v>
       </c>
     </row>
     <row r="22">
@@ -687,10 +687,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="n">
-        <v>0.0018821160899371</v>
+        <v>0.162555350705141</v>
       </c>
       <c r="C22" t="n">
-        <v>0.516947559712217</v>
+        <v>0.515055030560506</v>
       </c>
     </row>
     <row r="23">
@@ -698,10 +698,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="n">
-        <v>0.00160250732745357</v>
+        <v>0.233568655736157</v>
       </c>
       <c r="C23" t="n">
-        <v>0.755390405957713</v>
+        <v>0.749403991617224</v>
       </c>
     </row>
     <row r="24">
@@ -709,10 +709,10 @@
         <v>25</v>
       </c>
       <c r="B24" t="n">
-        <v>0.00180615577528142</v>
+        <v>0.145723933270154</v>
       </c>
       <c r="C24" t="n">
-        <v>0.574529469605555</v>
+        <v>0.576169097415042</v>
       </c>
     </row>
     <row r="25">
@@ -720,10 +720,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="n">
-        <v>0.00212273245810665</v>
+        <v>0.108861627629659</v>
       </c>
       <c r="C25" t="n">
-        <v>0.386242453558663</v>
+        <v>0.385076627920173</v>
       </c>
     </row>
     <row r="26">
@@ -731,10 +731,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="n">
-        <v>0.0136051287276264</v>
+        <v>0.266269000004038</v>
       </c>
       <c r="C26" t="n">
-        <v>0.869787836996433</v>
+        <v>0.863498245552782</v>
       </c>
     </row>
     <row r="27">
@@ -742,10 +742,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="n">
-        <v>0.0183512273078904</v>
+        <v>0.273581980872965</v>
       </c>
       <c r="C27" t="n">
-        <v>0.648213761760771</v>
+        <v>0.641524963502602</v>
       </c>
     </row>
     <row r="28">
@@ -753,10 +753,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="n">
-        <v>0.0115456789851813</v>
+        <v>0.227149154917128</v>
       </c>
       <c r="C28" t="n">
-        <v>0.866730154276343</v>
+        <v>0.861163482610652</v>
       </c>
     </row>
     <row r="29">
@@ -764,10 +764,10 @@
         <v>30</v>
       </c>
       <c r="B29" t="n">
-        <v>0.024929712001801</v>
+        <v>0.12165853248952</v>
       </c>
       <c r="C29" t="n">
-        <v>0.855217402768622</v>
+        <v>0.844209360580092</v>
       </c>
     </row>
     <row r="30">
@@ -775,10 +775,10 @@
         <v>31</v>
       </c>
       <c r="B30" t="n">
-        <v>0.00582005073071197</v>
+        <v>0.118353035793507</v>
       </c>
       <c r="C30" t="n">
-        <v>0.956139204944515</v>
+        <v>0.953956548204336</v>
       </c>
     </row>
     <row r="31">
@@ -786,10 +786,10 @@
         <v>32</v>
       </c>
       <c r="B31" t="n">
-        <v>0.00453709192327272</v>
+        <v>0.137988604712299</v>
       </c>
       <c r="C31" t="n">
-        <v>0.963057866656718</v>
+        <v>0.961908741558781</v>
       </c>
     </row>
     <row r="32">
@@ -797,10 +797,10 @@
         <v>33</v>
       </c>
       <c r="B32" t="n">
-        <v>0.0118441462606938</v>
+        <v>0.185996675990196</v>
       </c>
       <c r="C32" t="n">
-        <v>0.855177235585223</v>
+        <v>0.850898837610772</v>
       </c>
     </row>
     <row r="33">
@@ -808,10 +808,10 @@
         <v>34</v>
       </c>
       <c r="B33" t="n">
-        <v>0.00354216143923826</v>
+        <v>0.109601031603587</v>
       </c>
       <c r="C33" t="n">
-        <v>0.97880829015544</v>
+        <v>0.979626847934591</v>
       </c>
     </row>
     <row r="34">
@@ -819,10 +819,10 @@
         <v>35</v>
       </c>
       <c r="B34" t="n">
-        <v>0.00605909269741257</v>
+        <v>0.184657162511518</v>
       </c>
       <c r="C34" t="n">
-        <v>0.960629213958109</v>
+        <v>0.957876693509183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>